<commit_message>
deleted files and modified analyses
</commit_message>
<xml_diff>
--- a/data/quailsgate/2018 Pre-Harvest Grape Analysis.xlsx
+++ b/data/quailsgate/2018 Pre-Harvest Grape Analysis.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\QG-SHARED\Winery\2018 Harvest\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7978514B-BD0B-4E1E-935C-E569C6EE4164}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26819"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" tabRatio="941" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19940" yWindow="10000" windowWidth="25200" windowHeight="11780" tabRatio="941" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="CHARD" sheetId="1" r:id="rId1"/>
@@ -38,8 +32,11 @@
     <sheet name="GROWER SAMPLING" sheetId="13" r:id="rId23"/>
     <sheet name="Sheet18" sheetId="36" r:id="rId24"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -48,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="305">
   <si>
     <t>pH</t>
   </si>
@@ -704,9 +701,6 @@
     <t>18CHSYL MUSQ</t>
   </si>
   <si>
-    <t>09-14-2018</t>
-  </si>
-  <si>
     <t>18GNSHV</t>
   </si>
   <si>
@@ -831,9 +825,6 @@
   </si>
   <si>
     <t>18CAF2B3</t>
-  </si>
-  <si>
-    <t>09-27-2018</t>
   </si>
   <si>
     <t>18CAF1B7</t>
@@ -974,7 +965,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1070,7 +1061,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1122,7 +1113,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1316,31 +1307,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1048549"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1360,7 +1351,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>43347</v>
       </c>
@@ -1377,7 +1368,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>43347</v>
       </c>
@@ -1394,7 +1385,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>43347</v>
       </c>
@@ -1411,7 +1402,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>43348</v>
       </c>
@@ -1431,7 +1422,7 @@
         <v>41.1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>43348</v>
       </c>
@@ -1448,7 +1439,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>43348</v>
       </c>
@@ -1465,7 +1456,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>43350</v>
       </c>
@@ -1482,7 +1473,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
         <v>43350</v>
       </c>
@@ -1499,7 +1490,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
         <v>43350</v>
       </c>
@@ -1516,7 +1507,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>43355</v>
       </c>
@@ -1533,7 +1524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
         <v>43355</v>
       </c>
@@ -1550,7 +1541,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="2">
         <v>43355</v>
       </c>
@@ -1567,7 +1558,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="2">
         <v>43355</v>
       </c>
@@ -1584,7 +1575,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="2">
         <v>43356</v>
       </c>
@@ -1601,7 +1592,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="2">
         <v>43356</v>
       </c>
@@ -1618,7 +1609,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="2">
         <v>43356</v>
       </c>
@@ -1635,7 +1626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="2">
         <v>43356</v>
       </c>
@@ -1652,7 +1643,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="2">
         <v>43356</v>
       </c>
@@ -1669,7 +1660,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="2">
         <v>43357</v>
       </c>
@@ -1686,7 +1677,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="2">
         <v>43357</v>
       </c>
@@ -1703,7 +1694,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="2">
         <v>43357</v>
       </c>
@@ -1720,7 +1711,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="2">
         <v>43360</v>
       </c>
@@ -1737,7 +1728,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="2">
         <v>43360</v>
       </c>
@@ -1754,7 +1745,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="2">
         <v>43360</v>
       </c>
@@ -1771,12 +1762,12 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="2">
         <v>43360</v>
       </c>
       <c r="B26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C26">
         <v>21.3</v>
@@ -1788,12 +1779,12 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="2">
         <v>43360</v>
       </c>
       <c r="B27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C27">
         <v>22.8</v>
@@ -1805,12 +1796,12 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="2">
         <v>43360</v>
       </c>
       <c r="B28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C28">
         <v>21.1</v>
@@ -1822,12 +1813,12 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="2">
         <v>43362</v>
       </c>
       <c r="B29" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C29">
         <v>22.2</v>
@@ -1839,12 +1830,12 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="2">
         <v>43366</v>
       </c>
       <c r="B30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C30">
         <v>20.9</v>
@@ -1856,7 +1847,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="2">
         <v>43366</v>
       </c>
@@ -1873,12 +1864,12 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="2">
         <v>43366</v>
       </c>
       <c r="B32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C32">
         <v>23.5</v>
@@ -1890,12 +1881,12 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="2">
         <v>43366</v>
       </c>
       <c r="B33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C33">
         <v>22.3</v>
@@ -1907,12 +1898,12 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="2">
         <v>43367</v>
       </c>
       <c r="B34" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C34">
         <v>21</v>
@@ -1924,7 +1915,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="2">
         <v>43368</v>
       </c>
@@ -1941,18 +1932,18 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="2">
         <v>43372</v>
       </c>
       <c r="B36" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C36">
         <v>18.7</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="2">
         <v>43372</v>
       </c>
@@ -1969,7 +1960,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="2">
         <v>43372</v>
       </c>
@@ -1986,7 +1977,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="2">
         <v>43372</v>
       </c>
@@ -2003,12 +1994,12 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="2">
         <v>43372</v>
       </c>
       <c r="B40" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C40">
         <v>22.7</v>
@@ -2020,12 +2011,12 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="2">
         <v>43372</v>
       </c>
       <c r="B41" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C41">
         <v>22.8</v>
@@ -2037,12 +2028,12 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="2">
         <v>43372</v>
       </c>
       <c r="B42" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C42">
         <v>22.9</v>
@@ -2054,12 +2045,12 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="2">
         <v>43376</v>
       </c>
       <c r="B43" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C43">
         <v>21.3</v>
@@ -2071,12 +2062,12 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="2">
         <v>43376</v>
       </c>
       <c r="B44" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C44">
         <v>24.9</v>
@@ -2088,12 +2079,12 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="2">
         <v>43391</v>
       </c>
       <c r="B45" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C45">
         <v>22</v>
@@ -2105,12 +2096,12 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="2">
         <v>43391</v>
       </c>
       <c r="B46" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C46">
         <v>25</v>
@@ -2122,12 +2113,12 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="2">
         <v>43391</v>
       </c>
       <c r="B47" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C47">
         <v>24.3</v>
@@ -2139,32 +2130,37 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="1048549" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1048549" spans="1:1">
       <c r="A1048549" s="1">
         <v>43348</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2184,12 +2180,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>43362</v>
       </c>
       <c r="B2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C2">
         <v>24.2</v>
@@ -2201,12 +2197,12 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>43375</v>
       </c>
       <c r="B3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C3">
         <v>25.4</v>
@@ -2218,12 +2214,12 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>43375</v>
       </c>
       <c r="B4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C4">
         <v>25</v>
@@ -2235,12 +2231,12 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>43384</v>
       </c>
       <c r="B5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C5">
         <v>25.5</v>
@@ -2252,12 +2248,12 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>43384</v>
       </c>
       <c r="B6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C6">
         <v>24.4</v>
@@ -2269,12 +2265,12 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="2">
         <v>43384</v>
       </c>
       <c r="B7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C7">
         <v>24.9</v>
@@ -2286,12 +2282,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>43384</v>
       </c>
       <c r="B8" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C8">
         <v>24.8</v>
@@ -2305,24 +2301,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:F17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2338,13 +2339,10 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>192</v>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2">
+        <v>43355</v>
       </c>
       <c r="B2" t="s">
         <v>193</v>
@@ -2359,9 +2357,9 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>192</v>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2">
+        <v>43355</v>
       </c>
       <c r="B3" t="s">
         <v>194</v>
@@ -2376,12 +2374,12 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="2">
+        <v>43357</v>
+      </c>
+      <c r="B4" t="s">
         <v>218</v>
-      </c>
-      <c r="B4" t="s">
-        <v>219</v>
       </c>
       <c r="C4">
         <v>21.2</v>
@@ -2393,12 +2391,12 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>242</v>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2">
+        <v>43366</v>
       </c>
       <c r="B5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C5">
         <v>22.8</v>
@@ -2410,12 +2408,12 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>242</v>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2">
+        <v>43366</v>
       </c>
       <c r="B6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C6">
         <v>22.9</v>
@@ -2427,12 +2425,12 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>261</v>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2">
+        <v>43370</v>
       </c>
       <c r="B7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C7">
         <v>23.4</v>
@@ -2444,12 +2442,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>261</v>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2">
+        <v>43370</v>
       </c>
       <c r="B8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C8">
         <v>24.2</v>
@@ -2461,12 +2459,12 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="2">
         <v>43376</v>
       </c>
       <c r="B9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C9">
         <v>24.2</v>
@@ -2478,12 +2476,12 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="2">
         <v>43376</v>
       </c>
       <c r="B10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C10">
         <v>23.5</v>
@@ -2495,12 +2493,12 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="2">
         <v>43376</v>
       </c>
       <c r="B11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C11">
         <v>23.3</v>
@@ -2512,12 +2510,12 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="2">
         <v>43376</v>
       </c>
       <c r="B12" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C12">
         <v>23.3</v>
@@ -2529,12 +2527,12 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="2">
         <v>43376</v>
       </c>
       <c r="B13" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C13">
         <v>23.6</v>
@@ -2546,12 +2544,12 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="2">
         <v>43376</v>
       </c>
       <c r="B14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C14">
         <v>23.8</v>
@@ -2563,7 +2561,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="2">
         <v>43389</v>
       </c>
@@ -2580,7 +2578,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="2">
         <v>43389</v>
       </c>
@@ -2597,12 +2595,12 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="2">
         <v>43391</v>
       </c>
       <c r="B17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C17">
         <v>24.7</v>
@@ -2616,24 +2614,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2653,7 +2656,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>192</v>
       </c>
@@ -2670,7 +2673,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>192</v>
       </c>
@@ -2687,7 +2690,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>192</v>
       </c>
@@ -2704,7 +2707,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>192</v>
       </c>
@@ -2721,12 +2724,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" t="s">
         <v>242</v>
-      </c>
-      <c r="B6" t="s">
-        <v>243</v>
       </c>
       <c r="C6">
         <v>20.399999999999999</v>
@@ -2738,12 +2741,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C7">
         <v>18.8</v>
@@ -2755,12 +2758,12 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C8">
         <v>18.7</v>
@@ -2772,12 +2775,12 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B9" t="s">
         <v>288</v>
-      </c>
-      <c r="B9" t="s">
-        <v>290</v>
       </c>
       <c r="C9">
         <v>22.2</v>
@@ -2789,12 +2792,12 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
         <v>43389</v>
       </c>
       <c r="B10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C10">
         <v>21</v>
@@ -2806,12 +2809,12 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>43389</v>
       </c>
       <c r="B11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C11">
         <v>21.2</v>
@@ -2823,12 +2826,12 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
         <v>43389</v>
       </c>
       <c r="B12" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C12">
         <v>21.2</v>
@@ -2840,12 +2843,12 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="2">
         <v>43390</v>
       </c>
       <c r="B13" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C13">
         <v>21.8</v>
@@ -2859,23 +2862,28 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2895,7 +2903,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>192</v>
       </c>
@@ -2912,12 +2920,12 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>43362</v>
       </c>
       <c r="B3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C3">
         <v>21.8</v>
@@ -2929,12 +2937,12 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>43367</v>
       </c>
       <c r="B4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C4">
         <v>20.399999999999999</v>
@@ -2948,25 +2956,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2986,12 +2999,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>43360</v>
       </c>
       <c r="B2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C2">
         <v>22.4</v>
@@ -3003,12 +3016,12 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>43362</v>
       </c>
       <c r="B3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C3">
         <v>23.1</v>
@@ -3020,12 +3033,12 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>43368</v>
       </c>
       <c r="B4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C4">
         <v>22</v>
@@ -3037,12 +3050,12 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>43369</v>
       </c>
       <c r="B5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C5">
         <v>26.4</v>
@@ -3054,12 +3067,12 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>43372</v>
       </c>
       <c r="B6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C6">
         <v>25.6</v>
@@ -3071,12 +3084,12 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>43375</v>
       </c>
       <c r="B7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C7">
         <v>24</v>
@@ -3088,12 +3101,12 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>43378</v>
       </c>
       <c r="B8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C8">
         <v>25.2</v>
@@ -3105,12 +3118,12 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
         <v>43378</v>
       </c>
       <c r="B9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C9">
         <v>24.4</v>
@@ -3124,23 +3137,28 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3160,12 +3178,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>43367</v>
       </c>
       <c r="B2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C2">
         <v>19</v>
@@ -3177,12 +3195,12 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>43367</v>
       </c>
       <c r="B3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C3">
         <v>16.100000000000001</v>
@@ -3194,12 +3212,12 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>43368</v>
       </c>
       <c r="B4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C4">
         <v>17.899999999999999</v>
@@ -3211,12 +3229,12 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>43368</v>
       </c>
       <c r="B5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C5">
         <v>20</v>
@@ -3228,12 +3246,12 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>43371</v>
       </c>
       <c r="B6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C6">
         <v>19.2</v>
@@ -3241,26 +3259,31 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3280,12 +3303,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>43375</v>
       </c>
       <c r="B2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C2">
         <v>24.2</v>
@@ -3299,23 +3322,28 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEABA575-8C7E-44FE-B659-A852DA41BFD2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3335,12 +3363,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>43384</v>
       </c>
       <c r="B2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C2">
         <v>23.6</v>
@@ -3352,12 +3380,12 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>43384</v>
       </c>
       <c r="B3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C3">
         <v>24.6</v>
@@ -3369,12 +3397,12 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>43384</v>
       </c>
       <c r="B4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C4">
         <v>24.4</v>
@@ -3388,23 +3416,28 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3421,12 +3454,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>43366</v>
       </c>
       <c r="B2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C2">
         <v>21</v>
@@ -3438,12 +3471,12 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>43366</v>
       </c>
       <c r="B3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C3">
         <v>20.3</v>
@@ -3455,12 +3488,12 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>43367</v>
       </c>
       <c r="B4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C4">
         <v>21.7</v>
@@ -3472,7 +3505,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>43370</v>
       </c>
@@ -3489,12 +3522,12 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>43372</v>
       </c>
       <c r="B6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C6">
         <v>20.9</v>
@@ -3508,20 +3541,25 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A9B0F5-CE96-4C82-A285-BBBE3A139495}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3538,12 +3576,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C2">
         <v>23.4</v>
@@ -3555,9 +3593,9 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="B3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C3">
         <v>28.8</v>
@@ -3571,25 +3609,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView topLeftCell="A45" workbookViewId="0">
       <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3609,7 +3652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>43347</v>
       </c>
@@ -3626,7 +3669,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>43347</v>
       </c>
@@ -3646,7 +3689,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>43347</v>
       </c>
@@ -3666,7 +3709,7 @@
         <v>38.9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>43347</v>
       </c>
@@ -3683,7 +3726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>43347</v>
       </c>
@@ -3700,7 +3743,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>43348</v>
       </c>
@@ -3717,7 +3760,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>43348</v>
       </c>
@@ -3734,7 +3777,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
         <v>43348</v>
       </c>
@@ -3751,7 +3794,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
         <v>43348</v>
       </c>
@@ -3768,7 +3811,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>43348</v>
       </c>
@@ -3785,7 +3828,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
         <v>43348</v>
       </c>
@@ -3802,7 +3845,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="2">
         <v>43350</v>
       </c>
@@ -3822,7 +3865,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="2">
         <v>43350</v>
       </c>
@@ -3842,7 +3885,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="2">
         <v>43350</v>
       </c>
@@ -3859,7 +3902,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="2">
         <v>43350</v>
       </c>
@@ -3876,7 +3919,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="2">
         <v>43350</v>
       </c>
@@ -3893,7 +3936,7 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="2">
         <v>43350</v>
       </c>
@@ -3910,7 +3953,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="2">
         <v>43350</v>
       </c>
@@ -3927,7 +3970,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="2">
         <v>43350</v>
       </c>
@@ -3944,7 +3987,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="2">
         <v>43350</v>
       </c>
@@ -3964,7 +4007,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="2">
         <v>43350</v>
       </c>
@@ -3981,7 +4024,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="2">
         <v>43350</v>
       </c>
@@ -4001,7 +4044,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="2">
         <v>43350</v>
       </c>
@@ -4021,7 +4064,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="2">
         <v>43355</v>
       </c>
@@ -4038,7 +4081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="2">
         <v>43355</v>
       </c>
@@ -4055,7 +4098,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="2">
         <v>43355</v>
       </c>
@@ -4072,7 +4115,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="2">
         <v>43355</v>
       </c>
@@ -4089,7 +4132,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="2">
         <v>43355</v>
       </c>
@@ -4106,7 +4149,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="2">
         <v>43357</v>
       </c>
@@ -4126,7 +4169,7 @@
         <v>54.5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="2">
         <v>43357</v>
       </c>
@@ -4146,7 +4189,7 @@
         <v>45.3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="2">
         <v>43357</v>
       </c>
@@ -4166,7 +4209,7 @@
         <v>44.5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="2">
         <v>43357</v>
       </c>
@@ -4186,7 +4229,7 @@
         <v>46.6</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="2">
         <v>43357</v>
       </c>
@@ -4206,7 +4249,7 @@
         <v>50.5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="2">
         <v>43357</v>
       </c>
@@ -4226,7 +4269,7 @@
         <v>36.6</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="2">
         <v>43357</v>
       </c>
@@ -4246,7 +4289,7 @@
         <v>44.1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="2">
         <v>43357</v>
       </c>
@@ -4266,7 +4309,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="2">
         <v>43357</v>
       </c>
@@ -4286,7 +4329,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="2">
         <v>43357</v>
       </c>
@@ -4303,7 +4346,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="2">
         <v>43357</v>
       </c>
@@ -4320,7 +4363,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="2">
         <v>43360</v>
       </c>
@@ -4337,7 +4380,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="2">
         <v>43360</v>
       </c>
@@ -4354,12 +4397,12 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="2">
         <v>43360</v>
       </c>
       <c r="B43" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C43">
         <v>22.5</v>
@@ -4371,12 +4414,12 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" s="2">
         <v>43360</v>
       </c>
       <c r="B44" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C44">
         <v>23.3</v>
@@ -4388,12 +4431,12 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="2">
         <v>43360</v>
       </c>
       <c r="B45" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C45">
         <v>22.4</v>
@@ -4405,7 +4448,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="2">
         <v>43361</v>
       </c>
@@ -4425,12 +4468,12 @@
         <v>48.4</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="2">
         <v>43361</v>
       </c>
       <c r="B47" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C47">
         <v>22.9</v>
@@ -4442,7 +4485,7 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" s="2">
         <v>43361</v>
       </c>
@@ -4462,7 +4505,7 @@
         <v>49.1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" s="2">
         <v>43361</v>
       </c>
@@ -4482,12 +4525,12 @@
         <v>46.8</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="2">
         <v>43361</v>
       </c>
       <c r="B50" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C50">
         <v>24.4</v>
@@ -4502,12 +4545,12 @@
         <v>47.5</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" s="2">
         <v>43362</v>
       </c>
       <c r="B51" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C51">
         <v>20.8</v>
@@ -4519,7 +4562,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="2">
         <v>43366</v>
       </c>
@@ -4536,7 +4579,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="2">
         <v>43366</v>
       </c>
@@ -4553,7 +4596,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" s="2">
         <v>43366</v>
       </c>
@@ -4570,7 +4613,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" s="2">
         <v>43366</v>
       </c>
@@ -4587,7 +4630,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56" s="2">
         <v>43366</v>
       </c>
@@ -4604,12 +4647,12 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" s="2">
         <v>43367</v>
       </c>
       <c r="B57" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C57">
         <v>21.4</v>
@@ -4621,7 +4664,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" s="2">
         <v>43367</v>
       </c>
@@ -4638,7 +4681,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" s="2">
         <v>43367</v>
       </c>
@@ -4655,7 +4698,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" s="2">
         <v>43368</v>
       </c>
@@ -4672,7 +4715,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" s="2">
         <v>43368</v>
       </c>
@@ -4689,7 +4732,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" s="2">
         <v>43369</v>
       </c>
@@ -4706,7 +4749,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63" s="2">
         <v>43369</v>
       </c>
@@ -4723,12 +4766,12 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64" s="2">
         <v>43372</v>
       </c>
       <c r="B64" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C64">
         <v>22.8</v>
@@ -4740,12 +4783,12 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="2">
         <v>43372</v>
       </c>
       <c r="B65" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C65">
         <v>24.9</v>
@@ -4757,12 +4800,12 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="2">
         <v>43376</v>
       </c>
       <c r="B66" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C66">
         <v>21.6</v>
@@ -4774,12 +4817,12 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="2">
         <v>43376</v>
       </c>
       <c r="B67" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C67">
         <v>22.9</v>
@@ -4791,7 +4834,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" s="2">
         <v>43376</v>
       </c>
@@ -4808,12 +4851,12 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" s="2">
         <v>43384</v>
       </c>
       <c r="B69" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C69">
         <v>24.9</v>
@@ -4825,7 +4868,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="2">
         <v>43389</v>
       </c>
@@ -4842,12 +4885,12 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" s="2">
         <v>43389</v>
       </c>
       <c r="B71" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C71">
         <v>24</v>
@@ -4861,25 +4904,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4887,17 +4935,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -4911,13 +4959,13 @@
         <v>43372</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>43</v>
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -4928,7 +4976,7 @@
         <v>43388</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -4936,7 +4984,7 @@
         <v>43366</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -4950,7 +4998,7 @@
         <v>43355</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -4958,7 +5006,7 @@
         <v>43368</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -4972,12 +5020,12 @@
         <v>43372</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -4985,7 +5033,7 @@
         <v>43368</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -4999,7 +5047,7 @@
         <v>43372</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -5013,7 +5061,7 @@
         <v>43372</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -5021,12 +5069,12 @@
         <v>43369</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -5043,7 +5091,7 @@
         <v>43368</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -5051,7 +5099,7 @@
         <v>43347</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -5068,7 +5116,7 @@
         <v>43368</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -5088,7 +5136,7 @@
         <v>43366</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -5099,7 +5147,7 @@
         <v>43357</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -5110,7 +5158,7 @@
         <v>43357</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -5121,7 +5169,7 @@
         <v>43357</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -5132,7 +5180,7 @@
         <v>43357</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -5152,7 +5200,7 @@
         <v>43372</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -5163,7 +5211,7 @@
         <v>43357</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -5171,7 +5219,7 @@
         <v>43360</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -5182,17 +5230,17 @@
         <v>43348</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -5203,7 +5251,7 @@
         <v>43357</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -5214,7 +5262,7 @@
         <v>43357</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13">
       <c r="A34" t="s">
         <v>70</v>
       </c>
@@ -5228,7 +5276,7 @@
         <v>43361</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -5242,7 +5290,7 @@
         <v>43369</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -5256,7 +5304,7 @@
         <v>43369</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>73</v>
       </c>
@@ -5273,7 +5321,7 @@
         <v>43366</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -5284,7 +5332,7 @@
         <v>43356</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -5295,7 +5343,7 @@
         <v>43356</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -5312,7 +5360,7 @@
         <v>43366</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -5323,7 +5371,7 @@
         <v>43372</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -5337,7 +5385,7 @@
         <v>43372</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -5351,13 +5399,13 @@
         <v>43372</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13">
       <c r="A44" t="s">
         <v>80</v>
       </c>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13">
       <c r="A45" t="s">
         <v>81</v>
       </c>
@@ -5371,28 +5419,33 @@
         <v>43368</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13">
       <c r="A46" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -5400,7 +5453,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -5414,7 +5467,7 @@
         <v>43389</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>200</v>
       </c>
@@ -5428,7 +5481,7 @@
         <v>43389</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -5436,7 +5489,7 @@
         <v>43372</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -5450,7 +5503,7 @@
         <v>43389</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -5464,7 +5517,7 @@
         <v>43389</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>88</v>
       </c>
@@ -5475,7 +5528,7 @@
         <v>43389</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>89</v>
       </c>
@@ -5489,7 +5542,7 @@
         <v>43389</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -5500,7 +5553,7 @@
         <v>43372</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>91</v>
       </c>
@@ -5511,7 +5564,7 @@
         <v>43372</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>92</v>
       </c>
@@ -5522,12 +5575,12 @@
         <v>43372</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -5541,7 +5594,7 @@
         <v>43366</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -5558,7 +5611,7 @@
         <v>43366</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>96</v>
       </c>
@@ -5572,7 +5625,7 @@
         <v>43366</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>97</v>
       </c>
@@ -5580,7 +5633,7 @@
         <v>43350</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>98</v>
       </c>
@@ -5591,7 +5644,7 @@
         <v>43389</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -5602,7 +5655,7 @@
         <v>43389</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -5611,7 +5664,7 @@
         <v>43367</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -5625,7 +5678,7 @@
         <v>43389</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -5635,24 +5688,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="271" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="271" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>103</v>
       </c>
@@ -5663,7 +5721,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>105</v>
       </c>
@@ -5678,7 +5736,7 @@
         <v>43367</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="B3" t="s">
         <v>107</v>
       </c>
@@ -5690,7 +5748,7 @@
         <v>43367</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="B4" t="s">
         <v>108</v>
       </c>
@@ -5699,7 +5757,7 @@
         <v>43360</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="B5" t="s">
         <v>109</v>
       </c>
@@ -5708,7 +5766,7 @@
         <v>43360</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>110</v>
       </c>
@@ -5725,7 +5783,7 @@
         <v>43367</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" t="s">
         <v>112</v>
       </c>
@@ -5736,7 +5794,7 @@
         <v>43367</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="B9" t="s">
         <v>113</v>
       </c>
@@ -5747,7 +5805,7 @@
         <v>43367</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="B10" t="s">
         <v>114</v>
       </c>
@@ -5761,7 +5819,7 @@
         <v>43367</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="B11" t="s">
         <v>115</v>
       </c>
@@ -5775,7 +5833,7 @@
         <v>43367</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="B12" t="s">
         <v>116</v>
       </c>
@@ -5786,7 +5844,7 @@
         <v>43367</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="B13" t="s">
         <v>117</v>
       </c>
@@ -5800,7 +5858,7 @@
         <v>43367</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -5811,7 +5869,7 @@
         <v>43357</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="B16" t="s">
         <v>120</v>
       </c>
@@ -5819,22 +5877,22 @@
         <v>43357</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="B17" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="B18" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="B19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -5845,7 +5903,7 @@
         <v>43357</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="B22" t="s">
         <v>126</v>
       </c>
@@ -5853,7 +5911,7 @@
         <v>43357</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="B23" t="s">
         <v>127</v>
       </c>
@@ -5861,7 +5919,7 @@
         <v>43357</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="B24" t="s">
         <v>128</v>
       </c>
@@ -5869,7 +5927,7 @@
         <v>43357</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>129</v>
       </c>
@@ -5880,7 +5938,7 @@
         <v>43367</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="B27" t="s">
         <v>131</v>
       </c>
@@ -5888,7 +5946,7 @@
         <v>43367</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>132</v>
       </c>
@@ -5900,7 +5958,7 @@
       </c>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="B30" t="s">
         <v>134</v>
       </c>
@@ -5909,7 +5967,7 @@
       </c>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="B31" t="s">
         <v>135</v>
       </c>
@@ -5923,7 +5981,7 @@
         <v>43368</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="B32" t="s">
         <v>136</v>
       </c>
@@ -5936,25 +5994,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>103</v>
       </c>
@@ -5965,7 +6028,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -5983,7 +6046,7 @@
         <v>43389</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="B4" t="s">
         <v>139</v>
       </c>
@@ -5997,7 +6060,7 @@
         <v>43389</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="B5" t="s">
         <v>140</v>
       </c>
@@ -6014,7 +6077,7 @@
         <v>43389</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="B6" t="s">
         <v>141</v>
       </c>
@@ -6031,11 +6094,11 @@
         <v>43389</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="D7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>142</v>
       </c>
@@ -6050,7 +6113,7 @@
         <v>43391</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="B9" t="s">
         <v>144</v>
       </c>
@@ -6062,7 +6125,7 @@
         <v>43391</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="B10" t="s">
         <v>145</v>
       </c>
@@ -6074,10 +6137,10 @@
         <v>43391</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>146</v>
       </c>
@@ -6091,7 +6154,7 @@
         <v>43367</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="B13" t="s">
         <v>148</v>
       </c>
@@ -6102,7 +6165,7 @@
         <v>43367</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="B14" t="s">
         <v>149</v>
       </c>
@@ -6113,10 +6176,10 @@
         <v>43367</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>150</v>
       </c>
@@ -6125,10 +6188,10 @@
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>152</v>
       </c>
@@ -6140,7 +6203,7 @@
         <v>43360</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="B19" t="s">
         <v>154</v>
       </c>
@@ -6149,10 +6212,10 @@
         <v>43360</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>155</v>
       </c>
@@ -6164,7 +6227,7 @@
         <v>43360</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="B22" t="s">
         <v>157</v>
       </c>
@@ -6173,10 +6236,10 @@
         <v>43360</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>158</v>
       </c>
@@ -6191,10 +6254,10 @@
         <v>43370</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>160</v>
       </c>
@@ -6206,10 +6269,10 @@
         <v>43370</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>162</v>
       </c>
@@ -6223,10 +6286,10 @@
         <v>43363</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>164</v>
       </c>
@@ -6243,10 +6306,10 @@
         <v>43368</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>166</v>
       </c>
@@ -6255,13 +6318,13 @@
       </c>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7">
       <c r="B33" t="s">
         <v>168</v>
       </c>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7">
       <c r="B34" t="s">
         <v>169</v>
       </c>
@@ -6272,39 +6335,49 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="U37" sqref="U37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -6324,7 +6397,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>43349</v>
       </c>
@@ -6341,7 +6414,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>43355</v>
       </c>
@@ -6358,7 +6431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>43355</v>
       </c>
@@ -6375,12 +6448,12 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>43360</v>
       </c>
       <c r="B5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C5">
         <v>22</v>
@@ -6392,12 +6465,12 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>43360</v>
       </c>
       <c r="B6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C6">
         <v>20.3</v>
@@ -6409,12 +6482,12 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>43362</v>
       </c>
       <c r="B7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C7">
         <v>22</v>
@@ -6426,12 +6499,12 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>43363</v>
       </c>
       <c r="B8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C8">
         <v>21.7</v>
@@ -6443,7 +6516,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
         <v>43363</v>
       </c>
@@ -6460,12 +6533,12 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
         <v>43367</v>
       </c>
       <c r="B10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C10">
         <v>21.2</v>
@@ -6477,7 +6550,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>43367</v>
       </c>
@@ -6494,12 +6567,12 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
         <v>43367</v>
       </c>
       <c r="B12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C12">
         <v>23.3</v>
@@ -6511,7 +6584,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="2">
         <v>43367</v>
       </c>
@@ -6528,12 +6601,12 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="2">
         <v>43370</v>
       </c>
       <c r="B14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C14">
         <v>21.8</v>
@@ -6545,7 +6618,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="2">
         <v>43376</v>
       </c>
@@ -6562,12 +6635,12 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="2">
         <v>43376</v>
       </c>
       <c r="B16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C16">
         <v>21.9</v>
@@ -6579,12 +6652,12 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="2">
         <v>43376</v>
       </c>
       <c r="B17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C17">
         <v>22.8</v>
@@ -6596,7 +6669,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="2">
         <v>43376</v>
       </c>
@@ -6613,7 +6686,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="2">
         <v>43389</v>
       </c>
@@ -6632,25 +6705,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -6670,7 +6748,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>43349</v>
       </c>
@@ -6687,12 +6765,12 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>43362</v>
       </c>
       <c r="B3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C3">
         <v>22.5</v>
@@ -6704,12 +6782,12 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>43362</v>
       </c>
       <c r="B4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C4">
         <v>23.2</v>
@@ -6721,12 +6799,12 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>43368</v>
       </c>
       <c r="B5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C5">
         <v>23.5</v>
@@ -6738,12 +6816,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>43368</v>
       </c>
       <c r="B6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C6">
         <v>23.7</v>
@@ -6755,7 +6833,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>43369</v>
       </c>
@@ -6772,12 +6850,12 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>43372</v>
       </c>
       <c r="B8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C8">
         <v>21.4</v>
@@ -6789,12 +6867,12 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
         <v>43375</v>
       </c>
       <c r="B9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C9">
         <v>24.9</v>
@@ -6806,12 +6884,12 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
         <v>43375</v>
       </c>
       <c r="B10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C10">
         <v>25</v>
@@ -6823,12 +6901,12 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>43384</v>
       </c>
       <c r="B11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C11">
         <v>25.1</v>
@@ -6842,25 +6920,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -6880,7 +6963,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>43349</v>
       </c>
@@ -6897,12 +6980,12 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>43362</v>
       </c>
       <c r="B3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C3">
         <v>21.3</v>
@@ -6914,12 +6997,12 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>43368</v>
       </c>
       <c r="B4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C4">
         <v>23.8</v>
@@ -6933,25 +7016,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -6971,7 +7059,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>43348</v>
       </c>
@@ -6988,7 +7076,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>43355</v>
       </c>
@@ -7005,7 +7093,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>43355</v>
       </c>
@@ -7022,7 +7110,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>43356</v>
       </c>
@@ -7039,7 +7127,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>43357</v>
       </c>
@@ -7056,7 +7144,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>43357</v>
       </c>
@@ -7073,7 +7161,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>43357</v>
       </c>
@@ -7090,7 +7178,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
         <v>43357</v>
       </c>
@@ -7107,7 +7195,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
         <v>43357</v>
       </c>
@@ -7124,7 +7212,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>43357</v>
       </c>
@@ -7141,12 +7229,12 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
         <v>43360</v>
       </c>
       <c r="B12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C12">
         <v>19.399999999999999</v>
@@ -7158,7 +7246,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="2">
         <v>43367</v>
       </c>
@@ -7175,7 +7263,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>43368</v>
       </c>
@@ -7192,7 +7280,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="2">
         <v>43372</v>
       </c>
@@ -7209,7 +7297,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="2">
         <v>43376</v>
       </c>
@@ -7226,12 +7314,12 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="2">
         <v>43376</v>
       </c>
       <c r="B17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C17">
         <v>21.2</v>
@@ -7243,12 +7331,12 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="2">
         <v>43377</v>
       </c>
       <c r="B18" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C18">
         <v>23.4</v>
@@ -7262,24 +7350,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -7299,7 +7392,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>43347</v>
       </c>
@@ -7316,7 +7409,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>43350</v>
       </c>
@@ -7333,7 +7426,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>43355</v>
       </c>
@@ -7352,25 +7445,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -7390,7 +7488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>43347</v>
       </c>
@@ -7407,7 +7505,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>43347</v>
       </c>
@@ -7424,7 +7522,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>43348</v>
       </c>
@@ -7444,7 +7542,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>43348</v>
       </c>
@@ -7464,7 +7562,7 @@
         <v>57.1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>43349</v>
       </c>
@@ -7481,7 +7579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>43349</v>
       </c>
@@ -7500,24 +7598,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -7537,7 +7640,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>177</v>
       </c>
@@ -7554,7 +7657,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>177</v>
       </c>
@@ -7571,7 +7674,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>177</v>
       </c>
@@ -7588,9 +7691,9 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
@@ -7605,9 +7708,9 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
@@ -7622,12 +7725,12 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C7">
         <v>21.7</v>
@@ -7639,12 +7742,12 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>43389</v>
       </c>
       <c r="B8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C8">
         <v>21.3</v>
@@ -7656,12 +7759,12 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
         <v>43389</v>
       </c>
       <c r="B9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C9">
         <v>22.4</v>
@@ -7673,7 +7776,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
         <v>43389</v>
       </c>
@@ -7692,5 +7795,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>